<commit_message>
Started chaning folder structure
</commit_message>
<xml_diff>
--- a/Tables/He3_offset.xlsx
+++ b/Tables/He3_offset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderbackis/Documents/MultiGridAnalysisMesytec/Tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderbackis/Documents/MultiGridAnalysis/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D7B699-B217-2A4B-B5E4-392E763BAB9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FFFAC6-21C2-614D-AC5D-C78965D4258C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20720" yWindow="-5600" windowWidth="12840" windowHeight="19140" xr2:uid="{0B243B35-8923-414D-80B6-5F335095207C}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="12840" windowHeight="19140" xr2:uid="{0B243B35-8923-414D-80B6-5F335095207C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -663,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C9B202C-C072-5841-8706-FD22F81197F2}">
   <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -759,7 +759,7 @@
         <v>0.08</v>
       </c>
       <c r="C8">
-        <v>65</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -847,7 +847,7 @@
         <v>0.08</v>
       </c>
       <c r="C16">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>